<commit_message>
Adding updated input data
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/InputTestData.xlsx
+++ b/src/main/resources/testdata/InputTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srajp\eclipse-workspace\PlaywrightJavaProject\src\main\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srajp\eclipse-workspace\JavaPlaywright\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E24B71-11D8-42AA-AD3D-2C0FF49611B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA0037D-FAF1-4C6E-8906-0A679AD7BE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,20 +54,20 @@
     <t>Name</t>
   </si>
   <si>
-    <t>name.test11@gmail.com</t>
-  </si>
-  <si>
     <t>test@123</t>
   </si>
   <si>
     <t>1122334455</t>
+  </si>
+  <si>
+    <t>name.test12@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +79,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,16 +115,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,7 +408,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -435,27 +445,30 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{8EE5806E-23D8-4A62-806D-16F615F63381}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>